<commit_message>
style: 💄 update style
</commit_message>
<xml_diff>
--- a/fr/fr-adj.xlsx
+++ b/fr/fr-adj.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29080" windowHeight="13940" activeTab="1"/>
+    <workbookView windowWidth="29080" windowHeight="13940"/>
   </bookViews>
   <sheets>
     <sheet name="color" sheetId="1" r:id="rId1"/>
@@ -618,32 +618,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -770,7 +750,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -782,34 +762,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -894,18 +874,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1442,13 +1416,13 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" ht="17.55" spans="1:4">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1463,84 +1437,84 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" ht="17.55" spans="1:4">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1553,13 +1527,13 @@
   <sheetPr/>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" ht="17.55" spans="1:8">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1586,204 +1560,204 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" ht="17.55" spans="1:8">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>